<commit_message>
Calculate amounts of people for each data
</commit_message>
<xml_diff>
--- a/reports/IUP 2558.xlsx
+++ b/reports/IUP 2558.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zartr\Documents\GitHub\PSITProject16\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5085" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5085" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ตาราง 1" sheetId="29" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <sheet name="ตาราง 10" sheetId="38" r:id="rId10"/>
     <sheet name="ตาราง 11" sheetId="39" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="130">
   <si>
     <t>เพศ</t>
   </si>
@@ -580,7 +585,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -904,7 +909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -943,44 +948,80 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -991,54 +1032,18 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1135,6 +1140,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1407,7 +1415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1418,22 +1426,23 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="16.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="5"/>
+    <col min="4" max="4" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
@@ -1607,6 +1616,81 @@
       </c>
       <c r="H10" s="6">
         <v>6.7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="82">
+        <f>(D4/100)*4424</f>
+        <v>2486.2880000000005</v>
+      </c>
+      <c r="E12" s="82">
+        <f t="shared" ref="E12:G12" si="0">(E4/100)*4424</f>
+        <v>2304.904</v>
+      </c>
+      <c r="F12" s="82">
+        <f t="shared" si="0"/>
+        <v>1008.672</v>
+      </c>
+      <c r="G12" s="82">
+        <f t="shared" si="0"/>
+        <v>3521.5039999999999</v>
+      </c>
+      <c r="H12" s="82">
+        <f>(H4/100)*4424</f>
+        <v>389.31200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*5822</f>
+        <v>3138.058</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:I13" si="1">(E5/100)*5822</f>
+        <v>2311.3340000000003</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="1"/>
+        <v>1152.7560000000001</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="1"/>
+        <v>4884.6580000000004</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="1"/>
+        <v>489.04800000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="82">
+        <f>(D6/100)*188</f>
+        <v>83.847999999999999</v>
+      </c>
+      <c r="E14" s="82">
+        <f t="shared" ref="E14:H14" si="2">(E6/100)*188</f>
+        <v>97.948000000000008</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="2"/>
+        <v>35.72</v>
+      </c>
+      <c r="G14" s="82">
+        <f t="shared" si="2"/>
+        <v>163.184</v>
+      </c>
+      <c r="H14" s="82">
+        <f t="shared" si="2"/>
+        <v>10.904</v>
       </c>
     </row>
   </sheetData>
@@ -1622,7 +1706,7 @@
   </sheetPr>
   <dimension ref="B1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -1638,17 +1722,17 @@
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75">
+    <row r="1" spans="2:11" ht="18">
       <c r="B1" s="15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="19.5" thickBot="1">
+    <row r="2" spans="2:11" ht="18.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="19.5" thickBot="1">
+    <row r="3" spans="2:11" ht="18.75" thickBot="1">
       <c r="B3" s="78"/>
       <c r="C3" s="79"/>
       <c r="D3" s="2" t="s">
@@ -1676,7 +1760,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="19.5" thickBot="1">
+    <row r="4" spans="2:11" ht="18.75" thickBot="1">
       <c r="B4" s="65" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1792,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="19.5" thickBot="1">
+    <row r="5" spans="2:11" ht="18.75" thickBot="1">
       <c r="B5" s="66"/>
       <c r="C5" s="11" t="s">
         <v>1</v>
@@ -1738,7 +1822,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="19.5" thickBot="1">
+    <row r="6" spans="2:11" ht="18.75" thickBot="1">
       <c r="B6" s="67"/>
       <c r="C6" s="11" t="s">
         <v>20</v>
@@ -1768,7 +1852,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="19.5" thickBot="1">
+    <row r="7" spans="2:11" ht="18.75" thickBot="1">
       <c r="B7" s="57" t="s">
         <v>37</v>
       </c>
@@ -1800,7 +1884,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="19.5" thickBot="1">
+    <row r="8" spans="2:11" ht="18.75" thickBot="1">
       <c r="B8" s="58"/>
       <c r="C8" s="11" t="s">
         <v>39</v>
@@ -1830,7 +1914,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="19.5" thickBot="1">
+    <row r="9" spans="2:11" ht="18.75" thickBot="1">
       <c r="B9" s="58"/>
       <c r="C9" s="11" t="s">
         <v>40</v>
@@ -1860,7 +1944,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="19.5" thickBot="1">
+    <row r="10" spans="2:11" ht="18.75" thickBot="1">
       <c r="B10" s="59"/>
       <c r="C10" s="11" t="s">
         <v>41</v>
@@ -1907,7 +1991,7 @@
   </sheetPr>
   <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -1917,54 +2001,54 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="18.75">
+    <row r="2" spans="2:14" ht="18">
       <c r="B2" s="15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="19.5" thickBot="1">
+    <row r="3" spans="2:14" ht="18.75" thickBot="1">
       <c r="B3" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="123.75" thickBot="1">
+    <row r="4" spans="2:14" ht="192.75" thickBot="1">
       <c r="B4" s="80"/>
       <c r="C4" s="81"/>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="19.5" thickBot="1">
+    <row r="5" spans="2:14" ht="18.75" thickBot="1">
       <c r="B5" s="65" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +2089,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="19.5" thickBot="1">
+    <row r="6" spans="2:14" ht="18.75" thickBot="1">
       <c r="B6" s="66"/>
       <c r="C6" s="11" t="s">
         <v>1</v>
@@ -2044,7 +2128,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="19.5" thickBot="1">
+    <row r="7" spans="2:14" ht="18.75" thickBot="1">
       <c r="B7" s="67"/>
       <c r="C7" s="11" t="s">
         <v>20</v>
@@ -2083,7 +2167,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="19.5" thickBot="1">
+    <row r="8" spans="2:14" ht="18.75" thickBot="1">
       <c r="B8" s="57" t="s">
         <v>37</v>
       </c>
@@ -2124,7 +2208,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="19.5" thickBot="1">
+    <row r="9" spans="2:14" ht="18.75" thickBot="1">
       <c r="B9" s="58"/>
       <c r="C9" s="11" t="s">
         <v>39</v>
@@ -2163,7 +2247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="19.5" thickBot="1">
+    <row r="10" spans="2:14" ht="18.75" thickBot="1">
       <c r="B10" s="58"/>
       <c r="C10" s="11" t="s">
         <v>40</v>
@@ -2202,7 +2286,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="19.5" thickBot="1">
+    <row r="11" spans="2:14" ht="18.75" thickBot="1">
       <c r="B11" s="59"/>
       <c r="C11" s="11" t="s">
         <v>41</v>
@@ -2259,23 +2343,22 @@
   <dimension ref="B1:AG9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="5"/>
-    <col min="4" max="6" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="33" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="34" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
@@ -2284,56 +2367,56 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:33" ht="19.5" thickBot="1">
+    <row r="2" spans="2:33" ht="18.75" thickBot="1">
       <c r="B2" s="15"/>
     </row>
-    <row r="3" spans="2:33" ht="19.5" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="43" t="s">
+    <row r="3" spans="2:33" ht="18.75" thickBot="1">
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="43" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="43" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="43" t="s">
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="43" t="s">
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="45"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="32"/>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="33"/>
     </row>
     <row r="4" spans="2:33" s="1" customFormat="1" ht="84" customHeight="1" thickBot="1">
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="14" t="s">
         <v>24</v>
       </c>
@@ -2425,293 +2508,293 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:33" ht="19.5" thickBot="1">
+    <row r="5" spans="2:33" ht="18.75" thickBot="1">
       <c r="B5" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="30">
         <v>11.8</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="30">
         <v>17.3</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="30">
         <v>21.2</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="30">
         <v>11.8</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="30">
         <v>1.3</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="30">
         <v>0.3</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="30">
         <v>11.1</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="30">
         <v>9.1999999999999993</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="30">
         <v>20.3</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="30">
         <v>18.3</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="30">
         <v>3.9</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="30">
         <v>1.6</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="30">
         <v>8.1999999999999993</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="30">
         <v>6.5</v>
       </c>
-      <c r="R5" s="18">
+      <c r="R5" s="30">
         <v>13.1</v>
       </c>
-      <c r="S5" s="18">
+      <c r="S5" s="30">
         <v>7.8</v>
       </c>
-      <c r="T5" s="18">
+      <c r="T5" s="30">
         <v>1.3</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="30">
         <v>0.7</v>
       </c>
-      <c r="V5" s="18">
+      <c r="V5" s="30">
         <v>35.9</v>
       </c>
-      <c r="W5" s="18">
+      <c r="W5" s="30">
         <v>37.9</v>
       </c>
-      <c r="X5" s="18">
+      <c r="X5" s="30">
         <v>48.4</v>
       </c>
-      <c r="Y5" s="18">
+      <c r="Y5" s="30">
         <v>40.799999999999997</v>
       </c>
-      <c r="Z5" s="18">
+      <c r="Z5" s="30">
         <v>7.5</v>
       </c>
-      <c r="AA5" s="18">
+      <c r="AA5" s="30">
         <v>6.2</v>
       </c>
-      <c r="AB5" s="19">
+      <c r="AB5" s="18">
         <v>5.2</v>
       </c>
-      <c r="AC5" s="20">
+      <c r="AC5" s="19">
         <v>4.2</v>
       </c>
-      <c r="AD5" s="21">
+      <c r="AD5" s="20">
         <v>8.5</v>
       </c>
-      <c r="AE5" s="18">
+      <c r="AE5" s="30">
         <v>9.5</v>
       </c>
-      <c r="AF5" s="18">
+      <c r="AF5" s="30">
         <v>0.3</v>
       </c>
-      <c r="AG5" s="18">
+      <c r="AG5" s="30">
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="2:33" ht="19.5" thickBot="1">
+    <row r="6" spans="2:33" ht="18.75" thickBot="1">
       <c r="B6" s="41"/>
       <c r="C6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="30">
         <v>32.1</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="30">
         <v>33.5</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="30">
         <v>18.899999999999999</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="30">
         <v>15</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="30">
         <v>2.6</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="30">
         <v>1</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="30">
         <v>17.2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="30">
         <v>20.100000000000001</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="30">
         <v>22.5</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="30">
         <v>26.5</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="30">
         <v>4.5999999999999996</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="30">
         <v>1.2</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="30">
         <v>5.5</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="Q6" s="30">
         <v>6.4</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="30">
         <v>9.9</v>
       </c>
-      <c r="S6" s="18">
+      <c r="S6" s="30">
         <v>11.1</v>
       </c>
-      <c r="T6" s="18">
+      <c r="T6" s="30">
         <v>2</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="30">
         <v>1</v>
       </c>
-      <c r="V6" s="18">
+      <c r="V6" s="30">
         <v>45.9</v>
       </c>
-      <c r="W6" s="18">
+      <c r="W6" s="30">
         <v>49.1</v>
       </c>
-      <c r="X6" s="18">
+      <c r="X6" s="30">
         <v>58.3</v>
       </c>
-      <c r="Y6" s="18">
+      <c r="Y6" s="30">
         <v>59.4</v>
       </c>
-      <c r="Z6" s="18">
+      <c r="Z6" s="30">
         <v>11.2</v>
       </c>
-      <c r="AA6" s="18">
+      <c r="AA6" s="30">
         <v>8.1</v>
       </c>
-      <c r="AB6" s="19">
+      <c r="AB6" s="18">
         <v>2.4</v>
       </c>
-      <c r="AC6" s="20">
+      <c r="AC6" s="19">
         <v>1.7</v>
       </c>
-      <c r="AD6" s="21">
+      <c r="AD6" s="20">
         <v>4.3</v>
       </c>
-      <c r="AE6" s="18">
+      <c r="AE6" s="30">
         <v>6.6</v>
       </c>
-      <c r="AF6" s="18">
+      <c r="AF6" s="30">
         <v>0.7</v>
       </c>
-      <c r="AG6" s="18">
+      <c r="AG6" s="30">
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="19.5" thickBot="1">
+    <row r="7" spans="2:33" ht="18.75" thickBot="1">
       <c r="B7" s="41"/>
       <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="30">
         <v>53.4</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="30">
         <v>49.6</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="30">
         <v>16.8</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="30">
         <v>10.3</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="30">
         <v>1.2</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="30">
         <v>1.3</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="30">
         <v>21.9</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="30">
         <v>23.8</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="30">
         <v>17.3</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="30">
         <v>18.100000000000001</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="30">
         <v>2</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="30">
         <v>1.2</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="30">
         <v>8.1</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="30">
         <v>7.7</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="30">
         <v>14.7</v>
       </c>
-      <c r="S7" s="18">
+      <c r="S7" s="30">
         <v>17.8</v>
       </c>
-      <c r="T7" s="18">
+      <c r="T7" s="30">
         <v>1.4</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="30">
         <v>1.8</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="30">
         <v>44.5</v>
       </c>
-      <c r="W7" s="18">
+      <c r="W7" s="30">
         <v>43.1</v>
       </c>
-      <c r="X7" s="18">
+      <c r="X7" s="30">
         <v>55.7</v>
       </c>
-      <c r="Y7" s="18">
+      <c r="Y7" s="30">
         <v>52.4</v>
       </c>
-      <c r="Z7" s="18">
+      <c r="Z7" s="30">
         <v>5.7</v>
       </c>
-      <c r="AA7" s="18">
+      <c r="AA7" s="30">
         <v>10</v>
       </c>
-      <c r="AB7" s="19">
+      <c r="AB7" s="18">
         <v>1.3</v>
       </c>
-      <c r="AC7" s="20">
+      <c r="AC7" s="19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AD7" s="21">
+      <c r="AD7" s="20">
         <v>4</v>
       </c>
-      <c r="AE7" s="18">
+      <c r="AE7" s="30">
         <v>6.2</v>
       </c>
-      <c r="AF7" s="18">
+      <c r="AF7" s="30">
         <v>0.7</v>
       </c>
-      <c r="AG7" s="18">
+      <c r="AG7" s="30">
         <v>0.5</v>
       </c>
     </row>
@@ -2720,141 +2803,153 @@
       <c r="C8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="38">
         <v>52.7</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="38">
         <v>43.1</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="38">
         <v>16</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="38">
         <v>13.9</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="38">
         <v>1</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="38">
         <v>1</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="38">
         <v>17.5</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="38">
         <v>17</v>
       </c>
-      <c r="L8" s="37">
+      <c r="L8" s="38">
         <v>13.2</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="38">
         <v>15.9</v>
       </c>
-      <c r="N8" s="37">
+      <c r="N8" s="38">
         <v>1.3</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="38">
         <v>0.9</v>
       </c>
-      <c r="P8" s="37">
+      <c r="P8" s="38">
         <v>8.9</v>
       </c>
-      <c r="Q8" s="37">
+      <c r="Q8" s="38">
         <v>8</v>
       </c>
-      <c r="R8" s="37">
+      <c r="R8" s="38">
         <v>13.2</v>
       </c>
-      <c r="S8" s="37">
+      <c r="S8" s="38">
         <v>12.6</v>
       </c>
-      <c r="T8" s="37">
+      <c r="T8" s="38">
         <v>0.7</v>
       </c>
-      <c r="U8" s="37">
+      <c r="U8" s="38">
         <v>1.9</v>
       </c>
-      <c r="V8" s="37">
+      <c r="V8" s="38">
         <v>31.9</v>
       </c>
-      <c r="W8" s="37">
+      <c r="W8" s="38">
         <v>32.6</v>
       </c>
-      <c r="X8" s="37">
+      <c r="X8" s="38">
         <v>38.200000000000003</v>
       </c>
-      <c r="Y8" s="37">
+      <c r="Y8" s="38">
         <v>30.5</v>
       </c>
-      <c r="Z8" s="37">
+      <c r="Z8" s="38">
         <v>3.7</v>
       </c>
-      <c r="AA8" s="37">
+      <c r="AA8" s="38">
         <v>7</v>
       </c>
-      <c r="AB8" s="31">
+      <c r="AB8" s="43">
         <v>1.5</v>
       </c>
-      <c r="AC8" s="38">
+      <c r="AC8" s="48">
         <v>1</v>
       </c>
-      <c r="AD8" s="33">
+      <c r="AD8" s="45">
         <v>2.7</v>
       </c>
-      <c r="AE8" s="35">
+      <c r="AE8" s="46">
         <v>5</v>
       </c>
-      <c r="AF8" s="37">
+      <c r="AF8" s="38">
         <v>1.2</v>
       </c>
-      <c r="AG8" s="37">
+      <c r="AG8" s="38">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="19.5" thickBot="1">
+    <row r="9" spans="2:33" ht="18.75" thickBot="1">
       <c r="B9" s="42"/>
       <c r="C9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="34"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="32"/>
-      <c r="AC9" s="39"/>
-      <c r="AD9" s="34"/>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="39"/>
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="39"/>
+      <c r="AB9" s="44"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="39"/>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AB3:AG3"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="V3:AA3"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AE8:AE9"/>
+    <mergeCell ref="AF8:AF9"/>
+    <mergeCell ref="AG8:AG9"/>
+    <mergeCell ref="AC8:AC9"/>
+    <mergeCell ref="AA8:AA9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:Z9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="D8:D9"/>
@@ -2868,24 +2963,12 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="AE8:AE9"/>
-    <mergeCell ref="AF8:AF9"/>
-    <mergeCell ref="AG8:AG9"/>
-    <mergeCell ref="AC8:AC9"/>
+    <mergeCell ref="AB3:AG3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="V3:AA3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2896,29 +2979,30 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B2:I10"/>
+  <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="18.75">
+    <row r="2" spans="2:9" ht="18">
       <c r="B2" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="18.75">
+    <row r="3" spans="2:9" ht="18">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="7" t="s">
@@ -2940,7 +3024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="18.75">
+    <row r="4" spans="2:9" ht="18">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2966,7 +3050,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="18.75">
+    <row r="5" spans="2:9" ht="18">
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
         <v>53</v>
@@ -2990,7 +3074,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="18.75">
+    <row r="6" spans="2:9" ht="18">
       <c r="B6" s="10"/>
       <c r="C6" s="7" t="s">
         <v>54</v>
@@ -3014,7 +3098,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="18.75">
+    <row r="7" spans="2:9" ht="18">
       <c r="B7" s="8" t="s">
         <v>37</v>
       </c>
@@ -3040,7 +3124,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="18.75">
+    <row r="8" spans="2:9" ht="18">
       <c r="B8" s="9"/>
       <c r="C8" s="7" t="s">
         <v>56</v>
@@ -3064,7 +3148,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="18.75">
+    <row r="9" spans="2:9" ht="18">
       <c r="B9" s="9"/>
       <c r="C9" s="7" t="s">
         <v>57</v>
@@ -3088,7 +3172,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18.75">
+    <row r="10" spans="2:9" ht="18">
       <c r="B10" s="10"/>
       <c r="C10" s="7" t="s">
         <v>58</v>
@@ -3110,6 +3194,93 @@
       </c>
       <c r="I10" s="6">
         <v>19.7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="18">
+      <c r="C12" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="84">
+        <f>(D4/100)*4424</f>
+        <v>3813.4879999999998</v>
+      </c>
+      <c r="E12" s="84">
+        <f t="shared" ref="E12:I12" si="0">(E4/100)*4424</f>
+        <v>2552.6480000000001</v>
+      </c>
+      <c r="F12" s="84">
+        <f t="shared" si="0"/>
+        <v>698.99199999999996</v>
+      </c>
+      <c r="G12" s="84">
+        <f t="shared" si="0"/>
+        <v>137.14400000000001</v>
+      </c>
+      <c r="H12" s="84">
+        <f t="shared" si="0"/>
+        <v>601.66399999999999</v>
+      </c>
+      <c r="I12" s="84">
+        <f t="shared" si="0"/>
+        <v>1154.664</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18">
+      <c r="C13" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="84">
+        <f>(D5/100)*5822</f>
+        <v>5059.3180000000002</v>
+      </c>
+      <c r="E13" s="84">
+        <f t="shared" ref="E13:I13" si="1">(E5/100)*5822</f>
+        <v>3050.7280000000001</v>
+      </c>
+      <c r="F13" s="84">
+        <f t="shared" si="1"/>
+        <v>861.65600000000006</v>
+      </c>
+      <c r="G13" s="84">
+        <f t="shared" si="1"/>
+        <v>145.55000000000001</v>
+      </c>
+      <c r="H13" s="84">
+        <f t="shared" si="1"/>
+        <v>681.17399999999998</v>
+      </c>
+      <c r="I13" s="84">
+        <f t="shared" si="1"/>
+        <v>1659.2699999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="18">
+      <c r="C14" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="84">
+        <f>(D6/100)*188</f>
+        <v>171.26799999999997</v>
+      </c>
+      <c r="E14" s="84">
+        <f t="shared" ref="E14:I14" si="2">(E6/100)*188</f>
+        <v>72.192000000000007</v>
+      </c>
+      <c r="F14" s="84">
+        <f t="shared" si="2"/>
+        <v>52.451999999999991</v>
+      </c>
+      <c r="G14" s="84">
+        <f t="shared" si="2"/>
+        <v>7.8960000000000008</v>
+      </c>
+      <c r="H14" s="84">
+        <f t="shared" si="2"/>
+        <v>42.488</v>
+      </c>
+      <c r="I14" s="84">
+        <f t="shared" si="2"/>
+        <v>64.296000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -3122,17 +3293,24 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:O10"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C12" sqref="C12:O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="2" width="8.85546875" style="5"/>
     <col min="3" max="3" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="5"/>
+    <col min="4" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
@@ -3140,56 +3318,56 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="19.5" thickBot="1">
+    <row r="2" spans="2:15" ht="18.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="160.5" thickBot="1">
+    <row r="3" spans="2:15" ht="261.75" thickBot="1">
       <c r="B3" s="50"/>
       <c r="C3" s="51"/>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="19.5" thickBot="1">
+    <row r="4" spans="2:15" ht="18.75" thickBot="1">
       <c r="B4" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13">
@@ -3229,9 +3407,9 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="19.5" thickBot="1">
+    <row r="5" spans="2:15" ht="18.75" thickBot="1">
       <c r="B5" s="53"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="13">
@@ -3271,9 +3449,9 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="19.5" thickBot="1">
+    <row r="6" spans="2:15" ht="18.75" thickBot="1">
       <c r="B6" s="54"/>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="13">
@@ -3313,11 +3491,11 @@
         <v>52.4</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="19.5" thickBot="1">
+    <row r="7" spans="2:15" ht="18.75" thickBot="1">
       <c r="B7" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="13">
@@ -3357,9 +3535,9 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="19.5" thickBot="1">
+    <row r="8" spans="2:15" ht="18.75" thickBot="1">
       <c r="B8" s="53"/>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="13">
@@ -3399,9 +3577,9 @@
         <v>43.1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="19.5" thickBot="1">
+    <row r="9" spans="2:15" ht="18.75" thickBot="1">
       <c r="B9" s="53"/>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="13">
@@ -3441,9 +3619,9 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="19.5" thickBot="1">
+    <row r="10" spans="2:15" ht="18.75" thickBot="1">
       <c r="B10" s="54"/>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="13">
@@ -3481,6 +3659,165 @@
       </c>
       <c r="O10" s="13">
         <v>30.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="82">
+        <f>(D4/100)*4424</f>
+        <v>2442.0480000000002</v>
+      </c>
+      <c r="E12" s="82">
+        <f t="shared" ref="E12:O12" si="0">(E4/100)*4424</f>
+        <v>2915.4160000000002</v>
+      </c>
+      <c r="F12" s="82">
+        <f t="shared" si="0"/>
+        <v>3202.9760000000006</v>
+      </c>
+      <c r="G12" s="82">
+        <f t="shared" si="0"/>
+        <v>2265.0880000000002</v>
+      </c>
+      <c r="H12" s="82">
+        <f t="shared" si="0"/>
+        <v>685.72</v>
+      </c>
+      <c r="I12" s="82">
+        <f t="shared" si="0"/>
+        <v>1083.8799999999999</v>
+      </c>
+      <c r="J12" s="82">
+        <f t="shared" si="0"/>
+        <v>1336.048</v>
+      </c>
+      <c r="K12" s="82">
+        <f t="shared" si="0"/>
+        <v>482.21600000000001</v>
+      </c>
+      <c r="L12" s="82">
+        <f t="shared" si="0"/>
+        <v>836.13599999999985</v>
+      </c>
+      <c r="M12" s="82">
+        <f t="shared" si="0"/>
+        <v>1893.472</v>
+      </c>
+      <c r="N12" s="82">
+        <f t="shared" si="0"/>
+        <v>1030.7920000000001</v>
+      </c>
+      <c r="O12" s="82">
+        <f t="shared" si="0"/>
+        <v>1880.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*5822</f>
+        <v>2439.4180000000001</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:O13" si="1">(E5/100)*5822</f>
+        <v>3423.3359999999998</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="1"/>
+        <v>3743.5460000000003</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="1"/>
+        <v>2387.02</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="1"/>
+        <v>436.65</v>
+      </c>
+      <c r="I13" s="82">
+        <f t="shared" si="1"/>
+        <v>914.05399999999997</v>
+      </c>
+      <c r="J13" s="82">
+        <f t="shared" si="1"/>
+        <v>1408.924</v>
+      </c>
+      <c r="K13" s="82">
+        <f t="shared" si="1"/>
+        <v>494.87000000000006</v>
+      </c>
+      <c r="L13" s="82">
+        <f t="shared" si="1"/>
+        <v>1071.248</v>
+      </c>
+      <c r="M13" s="82">
+        <f t="shared" si="1"/>
+        <v>1560.296</v>
+      </c>
+      <c r="N13" s="82">
+        <f t="shared" si="1"/>
+        <v>751.03800000000001</v>
+      </c>
+      <c r="O13" s="82">
+        <f t="shared" si="1"/>
+        <v>2101.7419999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="82">
+        <f>(D6/100)*188</f>
+        <v>88.548000000000002</v>
+      </c>
+      <c r="E14" s="82">
+        <f t="shared" ref="E14:O14" si="2">(E6/100)*188</f>
+        <v>93.436000000000007</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="2"/>
+        <v>113.36399999999999</v>
+      </c>
+      <c r="G14" s="82">
+        <f t="shared" si="2"/>
+        <v>77.643999999999991</v>
+      </c>
+      <c r="H14" s="82">
+        <f t="shared" si="2"/>
+        <v>19.739999999999998</v>
+      </c>
+      <c r="I14" s="82">
+        <f t="shared" si="2"/>
+        <v>33.839999999999996</v>
+      </c>
+      <c r="J14" s="82">
+        <f t="shared" si="2"/>
+        <v>61.663999999999994</v>
+      </c>
+      <c r="K14" s="82">
+        <f t="shared" si="2"/>
+        <v>22.936</v>
+      </c>
+      <c r="L14" s="82">
+        <f t="shared" si="2"/>
+        <v>34.591999999999999</v>
+      </c>
+      <c r="M14" s="82">
+        <f t="shared" si="2"/>
+        <v>90.051999999999992</v>
+      </c>
+      <c r="N14" s="82">
+        <f t="shared" si="2"/>
+        <v>57.716000000000001</v>
+      </c>
+      <c r="O14" s="82">
+        <f t="shared" si="2"/>
+        <v>98.512</v>
       </c>
     </row>
   </sheetData>
@@ -3498,13 +3835,13 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:O10"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="16384" width="8.85546875" style="5"/>
   </cols>
@@ -3514,52 +3851,52 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="19.5" thickBot="1">
+    <row r="2" spans="2:15" ht="18.75" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="160.5" thickBot="1">
+    <row r="3" spans="2:15" ht="261.75" thickBot="1">
       <c r="B3" s="55"/>
       <c r="C3" s="56"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="19.5" thickBot="1">
+    <row r="4" spans="2:15" ht="18.75" thickBot="1">
       <c r="B4" s="57" t="s">
         <v>0</v>
       </c>
@@ -3603,7 +3940,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="19.5" thickBot="1">
+    <row r="5" spans="2:15" ht="18.75" thickBot="1">
       <c r="B5" s="58"/>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -3645,7 +3982,7 @@
         <v>44.8</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="19.5" thickBot="1">
+    <row r="6" spans="2:15" ht="18.75" thickBot="1">
       <c r="B6" s="59"/>
       <c r="C6" s="3" t="s">
         <v>20</v>
@@ -3687,7 +4024,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="19.5" thickBot="1">
+    <row r="7" spans="2:15" ht="18.75" thickBot="1">
       <c r="B7" s="57" t="s">
         <v>37</v>
       </c>
@@ -3731,7 +4068,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="19.5" thickBot="1">
+    <row r="8" spans="2:15" ht="18.75" thickBot="1">
       <c r="B8" s="58"/>
       <c r="C8" s="3" t="s">
         <v>39</v>
@@ -3773,7 +4110,7 @@
         <v>43.1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="19.5" thickBot="1">
+    <row r="9" spans="2:15" ht="18.75" thickBot="1">
       <c r="B9" s="58"/>
       <c r="C9" s="3" t="s">
         <v>40</v>
@@ -3815,7 +4152,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="19.5" thickBot="1">
+    <row r="10" spans="2:15" ht="18.75" thickBot="1">
       <c r="B10" s="59"/>
       <c r="C10" s="3" t="s">
         <v>41</v>
@@ -3855,6 +4192,165 @@
       </c>
       <c r="O10" s="4">
         <v>30.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="82">
+        <f>(D4/100)*4424</f>
+        <v>3618.8319999999999</v>
+      </c>
+      <c r="E12" s="82">
+        <f t="shared" ref="E12:O12" si="0">(E4/100)*4424</f>
+        <v>1902.32</v>
+      </c>
+      <c r="F12" s="82">
+        <f t="shared" si="0"/>
+        <v>2517.2559999999999</v>
+      </c>
+      <c r="G12" s="82">
+        <f t="shared" si="0"/>
+        <v>2371.2640000000001</v>
+      </c>
+      <c r="H12" s="82">
+        <f t="shared" si="0"/>
+        <v>725.53599999999994</v>
+      </c>
+      <c r="I12" s="82">
+        <f t="shared" si="0"/>
+        <v>1247.568</v>
+      </c>
+      <c r="J12" s="82">
+        <f t="shared" si="0"/>
+        <v>982.12800000000004</v>
+      </c>
+      <c r="K12" s="82">
+        <f t="shared" si="0"/>
+        <v>389.31200000000001</v>
+      </c>
+      <c r="L12" s="82">
+        <f t="shared" si="0"/>
+        <v>681.29599999999994</v>
+      </c>
+      <c r="M12" s="82">
+        <f t="shared" si="0"/>
+        <v>1159.088</v>
+      </c>
+      <c r="N12" s="82">
+        <f t="shared" si="0"/>
+        <v>1154.664</v>
+      </c>
+      <c r="O12" s="82">
+        <f t="shared" si="0"/>
+        <v>1583.7919999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*5822</f>
+        <v>4977.8099999999995</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:O13" si="1">(E5/100)*5822</f>
+        <v>2171.6059999999998</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="1"/>
+        <v>3434.98</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="1"/>
+        <v>3143.88</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="1"/>
+        <v>605.48800000000006</v>
+      </c>
+      <c r="I13" s="82">
+        <f t="shared" si="1"/>
+        <v>1339.06</v>
+      </c>
+      <c r="J13" s="82">
+        <f t="shared" si="1"/>
+        <v>1764.066</v>
+      </c>
+      <c r="K13" s="82">
+        <f t="shared" si="1"/>
+        <v>634.59799999999996</v>
+      </c>
+      <c r="L13" s="82">
+        <f t="shared" si="1"/>
+        <v>861.65600000000006</v>
+      </c>
+      <c r="M13" s="82">
+        <f t="shared" si="1"/>
+        <v>1606.8720000000001</v>
+      </c>
+      <c r="N13" s="82">
+        <f t="shared" si="1"/>
+        <v>1723.3120000000001</v>
+      </c>
+      <c r="O13" s="82">
+        <f t="shared" si="1"/>
+        <v>2608.2559999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="82">
+        <f>(D6/100)*188</f>
+        <v>170.14000000000001</v>
+      </c>
+      <c r="E14" s="82">
+        <f t="shared" ref="E14:O14" si="2">(E6/100)*188</f>
+        <v>76.516000000000005</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="2"/>
+        <v>116.372</v>
+      </c>
+      <c r="G14" s="82">
+        <f t="shared" si="2"/>
+        <v>107.34800000000001</v>
+      </c>
+      <c r="H14" s="82">
+        <f t="shared" si="2"/>
+        <v>19.739999999999998</v>
+      </c>
+      <c r="I14" s="82">
+        <f t="shared" si="2"/>
+        <v>58.655999999999999</v>
+      </c>
+      <c r="J14" s="82">
+        <f t="shared" si="2"/>
+        <v>54.708000000000006</v>
+      </c>
+      <c r="K14" s="82">
+        <f t="shared" si="2"/>
+        <v>24.816000000000003</v>
+      </c>
+      <c r="L14" s="82">
+        <f t="shared" si="2"/>
+        <v>33.652000000000001</v>
+      </c>
+      <c r="M14" s="82">
+        <f t="shared" si="2"/>
+        <v>75.2</v>
+      </c>
+      <c r="N14" s="82">
+        <f t="shared" si="2"/>
+        <v>67.679999999999993</v>
+      </c>
+      <c r="O14" s="82">
+        <f t="shared" si="2"/>
+        <v>93.436000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -3872,10 +4368,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:I9"/>
+  <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3885,34 +4381,34 @@
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="19.5" thickBot="1">
+    <row r="1" spans="2:15" ht="18.75" thickBot="1">
       <c r="B1" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="38.25" thickBot="1">
+    <row r="2" spans="2:15" ht="36.75" thickBot="1">
       <c r="B2" s="60"/>
       <c r="C2" s="61"/>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="19.5" thickBot="1">
+    <row r="3" spans="2:15" ht="18.75" thickBot="1">
       <c r="B3" s="57" t="s">
         <v>0</v>
       </c>
@@ -3922,7 +4418,7 @@
       <c r="D3" s="4">
         <v>92</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>60.2</v>
       </c>
       <c r="F3" s="4">
@@ -3938,7 +4434,7 @@
         <v>87.3</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="19.5" thickBot="1">
+    <row r="4" spans="2:15" ht="18.75" thickBot="1">
       <c r="B4" s="58"/>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -3946,7 +4442,7 @@
       <c r="D4" s="4">
         <v>92.6</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>72.8</v>
       </c>
       <c r="F4" s="4">
@@ -3962,7 +4458,7 @@
         <v>89.3</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="19.5" thickBot="1">
+    <row r="5" spans="2:15" ht="18.75" thickBot="1">
       <c r="B5" s="59"/>
       <c r="C5" s="3" t="s">
         <v>20</v>
@@ -3970,7 +4466,7 @@
       <c r="D5" s="4">
         <v>97.4</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <v>58.9</v>
       </c>
       <c r="F5" s="4">
@@ -3986,7 +4482,7 @@
         <v>87.4</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="19.5" thickBot="1">
+    <row r="6" spans="2:15" ht="18.75" thickBot="1">
       <c r="B6" s="57" t="s">
         <v>37</v>
       </c>
@@ -3996,7 +4492,7 @@
       <c r="D6" s="4">
         <v>91.5</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>66</v>
       </c>
       <c r="F6" s="4">
@@ -4012,7 +4508,7 @@
         <v>71.900000000000006</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="19.5" thickBot="1">
+    <row r="7" spans="2:15" ht="18.75" thickBot="1">
       <c r="B7" s="58"/>
       <c r="C7" s="3" t="s">
         <v>39</v>
@@ -4020,7 +4516,7 @@
       <c r="D7" s="4">
         <v>94.9</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>64.900000000000006</v>
       </c>
       <c r="F7" s="4">
@@ -4036,7 +4532,7 @@
         <v>88.3</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="19.5" thickBot="1">
+    <row r="8" spans="2:15" ht="18.75" thickBot="1">
       <c r="B8" s="58"/>
       <c r="C8" s="3" t="s">
         <v>40</v>
@@ -4044,7 +4540,7 @@
       <c r="D8" s="4">
         <v>90.5</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="27">
         <v>70.900000000000006</v>
       </c>
       <c r="F8" s="4">
@@ -4060,7 +4556,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="19.5" thickBot="1">
+    <row r="9" spans="2:15" ht="18.75" thickBot="1">
       <c r="B9" s="62"/>
       <c r="C9" s="3" t="s">
         <v>69</v>
@@ -4068,7 +4564,7 @@
       <c r="D9" s="4">
         <v>75.599999999999994</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>75.7</v>
       </c>
       <c r="F9" s="4">
@@ -4083,6 +4579,111 @@
       <c r="I9" s="4">
         <v>81.599999999999994</v>
       </c>
+    </row>
+    <row r="11" spans="2:15" ht="18">
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="82">
+        <f>(D3/100)*4424</f>
+        <v>4070.0800000000004</v>
+      </c>
+      <c r="E11" s="82">
+        <f t="shared" ref="E11:H11" si="0">(E3/100)*4424</f>
+        <v>2663.248</v>
+      </c>
+      <c r="F11" s="82">
+        <f t="shared" si="0"/>
+        <v>778.62400000000002</v>
+      </c>
+      <c r="G11" s="82">
+        <f t="shared" si="0"/>
+        <v>1442.2240000000002</v>
+      </c>
+      <c r="H11" s="82">
+        <f t="shared" si="0"/>
+        <v>159.26400000000001</v>
+      </c>
+      <c r="I11" s="82">
+        <f>(I3/100)*4424</f>
+        <v>3862.152</v>
+      </c>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+    </row>
+    <row r="12" spans="2:15" ht="18">
+      <c r="C12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="82">
+        <f>(D4/100)*5822</f>
+        <v>5391.1719999999996</v>
+      </c>
+      <c r="E12" s="82">
+        <f t="shared" ref="E12:H12" si="1">(E4/100)*5822</f>
+        <v>4238.4160000000002</v>
+      </c>
+      <c r="F12" s="82">
+        <f t="shared" si="1"/>
+        <v>1146.934</v>
+      </c>
+      <c r="G12" s="82">
+        <f t="shared" si="1"/>
+        <v>2666.4759999999997</v>
+      </c>
+      <c r="H12" s="82">
+        <f t="shared" si="1"/>
+        <v>192.126</v>
+      </c>
+      <c r="I12" s="82">
+        <f>(I4/100)*5822</f>
+        <v>5199.0460000000003</v>
+      </c>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+    </row>
+    <row r="13" spans="2:15" ht="18">
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*188</f>
+        <v>183.11200000000002</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:H13" si="2">(E5/100)*188</f>
+        <v>110.732</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="2"/>
+        <v>66.36399999999999</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="2"/>
+        <v>111.86</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="2"/>
+        <v>9.9640000000000004</v>
+      </c>
+      <c r="I13" s="82">
+        <f>(I5/100)*188</f>
+        <v>164.31200000000001</v>
+      </c>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4099,10 +4700,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:J11"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4111,17 +4712,17 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.25">
+    <row r="1" spans="2:15" ht="23.25">
       <c r="B1" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="19.5" thickBot="1">
+    <row r="2" spans="2:15" ht="18.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="151.9" customHeight="1">
+    <row r="3" spans="2:15" ht="151.9" customHeight="1">
       <c r="B3" s="68"/>
       <c r="C3" s="69"/>
       <c r="D3" s="63" t="s">
@@ -4146,7 +4747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="24.6" customHeight="1" thickBot="1">
+    <row r="4" spans="2:15" ht="24.6" customHeight="1" thickBot="1">
       <c r="B4" s="70"/>
       <c r="C4" s="71"/>
       <c r="D4" s="64"/>
@@ -4157,7 +4758,7 @@
       <c r="I4" s="64"/>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="2:10" ht="19.5" thickBot="1">
+    <row r="5" spans="2:15" ht="18.75" thickBot="1">
       <c r="B5" s="65" t="s">
         <v>0</v>
       </c>
@@ -4186,7 +4787,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="19.5" thickBot="1">
+    <row r="6" spans="2:15" ht="18.75" thickBot="1">
       <c r="B6" s="66"/>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -4213,7 +4814,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="19.5" thickBot="1">
+    <row r="7" spans="2:15" ht="18.75" thickBot="1">
       <c r="B7" s="67"/>
       <c r="C7" s="3" t="s">
         <v>20</v>
@@ -4240,7 +4841,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="19.5" thickBot="1">
+    <row r="8" spans="2:15" ht="18.75" thickBot="1">
       <c r="B8" s="57" t="s">
         <v>37</v>
       </c>
@@ -4269,7 +4870,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="19.5" thickBot="1">
+    <row r="9" spans="2:15" ht="18.75" thickBot="1">
       <c r="B9" s="58"/>
       <c r="C9" s="3" t="s">
         <v>77</v>
@@ -4296,7 +4897,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="19.5" thickBot="1">
+    <row r="10" spans="2:15" ht="18.75" thickBot="1">
       <c r="B10" s="58"/>
       <c r="C10" s="3" t="s">
         <v>78</v>
@@ -4323,7 +4924,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="19.5" thickBot="1">
+    <row r="11" spans="2:15" ht="18.75" thickBot="1">
       <c r="B11" s="59"/>
       <c r="C11" s="3" t="s">
         <v>41</v>
@@ -4349,6 +4950,120 @@
       <c r="J11" s="4">
         <v>3.7</v>
       </c>
+    </row>
+    <row r="13" spans="2:15" ht="18">
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*4424</f>
+        <v>1645.7280000000003</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:O13" si="0">(E5/100)*4424</f>
+        <v>2486.2880000000005</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="0"/>
+        <v>1796.1440000000002</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="0"/>
+        <v>2495.136</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="0"/>
+        <v>650.32799999999997</v>
+      </c>
+      <c r="I13" s="82">
+        <f t="shared" si="0"/>
+        <v>1340.472</v>
+      </c>
+      <c r="J13" s="82">
+        <f t="shared" si="0"/>
+        <v>207.928</v>
+      </c>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+    </row>
+    <row r="14" spans="2:15" ht="18">
+      <c r="C14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="82">
+        <f>(D6/100)*5822</f>
+        <v>1746.6</v>
+      </c>
+      <c r="E14" s="82">
+        <f t="shared" ref="E14:O14" si="1">(E6/100)*5822</f>
+        <v>2922.6440000000002</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="1"/>
+        <v>1723.3120000000001</v>
+      </c>
+      <c r="G14" s="82">
+        <f t="shared" si="1"/>
+        <v>3539.7759999999998</v>
+      </c>
+      <c r="H14" s="82">
+        <f t="shared" si="1"/>
+        <v>1403.1020000000001</v>
+      </c>
+      <c r="I14" s="82">
+        <f t="shared" si="1"/>
+        <v>2154.14</v>
+      </c>
+      <c r="J14" s="82">
+        <f t="shared" si="1"/>
+        <v>296.92199999999997</v>
+      </c>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+    </row>
+    <row r="15" spans="2:15" ht="18">
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="82">
+        <f>(D7/100)*188</f>
+        <v>64.108000000000004</v>
+      </c>
+      <c r="E15" s="82">
+        <f t="shared" ref="E15:O15" si="2">(E7/100)*188</f>
+        <v>105.468</v>
+      </c>
+      <c r="F15" s="82">
+        <f t="shared" si="2"/>
+        <v>75.576000000000008</v>
+      </c>
+      <c r="G15" s="82">
+        <f t="shared" si="2"/>
+        <v>111.10799999999999</v>
+      </c>
+      <c r="H15" s="82">
+        <f t="shared" si="2"/>
+        <v>55.459999999999994</v>
+      </c>
+      <c r="I15" s="82">
+        <f t="shared" si="2"/>
+        <v>82.531999999999996</v>
+      </c>
+      <c r="J15" s="82">
+        <f t="shared" si="2"/>
+        <v>9.9640000000000004</v>
+      </c>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4372,10 +5087,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:M10"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C12" sqref="C12:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4384,51 +5099,51 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="18.75">
+    <row r="1" spans="2:15" ht="18">
       <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="19.5" thickBot="1">
+    <row r="2" spans="2:15" ht="18.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="90" thickBot="1">
+    <row r="3" spans="2:15" ht="149.25" thickBot="1">
       <c r="B3" s="72"/>
       <c r="C3" s="73"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="19.5" thickBot="1">
+    <row r="4" spans="2:15" ht="18.75" thickBot="1">
       <c r="B4" s="65" t="s">
         <v>0</v>
       </c>
@@ -4466,7 +5181,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="19.5" thickBot="1">
+    <row r="5" spans="2:15" ht="18.75" thickBot="1">
       <c r="B5" s="66"/>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -4502,7 +5217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="19.5" thickBot="1">
+    <row r="6" spans="2:15" ht="18.75" thickBot="1">
       <c r="B6" s="67"/>
       <c r="C6" s="3" t="s">
         <v>20</v>
@@ -4538,7 +5253,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="19.5" thickBot="1">
+    <row r="7" spans="2:15" ht="18.75" thickBot="1">
       <c r="B7" s="57" t="s">
         <v>37</v>
       </c>
@@ -4576,7 +5291,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="19.5" thickBot="1">
+    <row r="8" spans="2:15" ht="18.75" thickBot="1">
       <c r="B8" s="58"/>
       <c r="C8" s="3" t="s">
         <v>39</v>
@@ -4612,7 +5327,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="19.5" thickBot="1">
+    <row r="9" spans="2:15" ht="18.75" thickBot="1">
       <c r="B9" s="58"/>
       <c r="C9" s="3" t="s">
         <v>40</v>
@@ -4648,7 +5363,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="19.5" thickBot="1">
+    <row r="10" spans="2:15" ht="18.75" thickBot="1">
       <c r="B10" s="59"/>
       <c r="C10" s="3" t="s">
         <v>41</v>
@@ -4683,6 +5398,147 @@
       <c r="M10" s="4">
         <v>39</v>
       </c>
+    </row>
+    <row r="12" spans="2:15" ht="18">
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="82">
+        <f>(D4/100)*4424</f>
+        <v>1097.152</v>
+      </c>
+      <c r="E12" s="82">
+        <f t="shared" ref="E12:O12" si="0">(E4/100)*4424</f>
+        <v>115.02400000000002</v>
+      </c>
+      <c r="F12" s="82">
+        <f t="shared" si="0"/>
+        <v>650.32799999999997</v>
+      </c>
+      <c r="G12" s="82">
+        <f t="shared" si="0"/>
+        <v>641.4799999999999</v>
+      </c>
+      <c r="H12" s="82">
+        <f t="shared" si="0"/>
+        <v>2061.5840000000003</v>
+      </c>
+      <c r="I12" s="82">
+        <f t="shared" si="0"/>
+        <v>132.72</v>
+      </c>
+      <c r="J12" s="82">
+        <f t="shared" si="0"/>
+        <v>460.09600000000006</v>
+      </c>
+      <c r="K12" s="82">
+        <f t="shared" si="0"/>
+        <v>539.72799999999995</v>
+      </c>
+      <c r="L12" s="82">
+        <f t="shared" si="0"/>
+        <v>1154.664</v>
+      </c>
+      <c r="M12" s="82">
+        <f t="shared" si="0"/>
+        <v>1234.2959999999998</v>
+      </c>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+    </row>
+    <row r="13" spans="2:15" ht="18">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*5822</f>
+        <v>3143.88</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:O13" si="1">(E5/100)*5822</f>
+        <v>366.786</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="1"/>
+        <v>2072.6320000000001</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="1"/>
+        <v>716.10600000000011</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="1"/>
+        <v>937.34199999999998</v>
+      </c>
+      <c r="I13" s="82">
+        <f t="shared" si="1"/>
+        <v>308.56599999999997</v>
+      </c>
+      <c r="J13" s="82">
+        <f t="shared" si="1"/>
+        <v>291.10000000000002</v>
+      </c>
+      <c r="K13" s="82">
+        <f t="shared" si="1"/>
+        <v>698.64</v>
+      </c>
+      <c r="L13" s="82">
+        <f t="shared" si="1"/>
+        <v>1036.316</v>
+      </c>
+      <c r="M13" s="82">
+        <f t="shared" si="1"/>
+        <v>1571.94</v>
+      </c>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+    </row>
+    <row r="14" spans="2:15" ht="18">
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="82">
+        <f>(D6/100)*188</f>
+        <v>95.504000000000005</v>
+      </c>
+      <c r="E14" s="82">
+        <f t="shared" ref="E14:O14" si="2">(E6/100)*188</f>
+        <v>9.9640000000000004</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="2"/>
+        <v>62.603999999999992</v>
+      </c>
+      <c r="G14" s="82">
+        <f t="shared" si="2"/>
+        <v>7.1440000000000001</v>
+      </c>
+      <c r="H14" s="82">
+        <f t="shared" si="2"/>
+        <v>54.144000000000005</v>
+      </c>
+      <c r="I14" s="82">
+        <f t="shared" si="2"/>
+        <v>2.82</v>
+      </c>
+      <c r="J14" s="82">
+        <f t="shared" si="2"/>
+        <v>7.1440000000000001</v>
+      </c>
+      <c r="K14" s="82">
+        <f t="shared" si="2"/>
+        <v>35.531999999999996</v>
+      </c>
+      <c r="L14" s="82">
+        <f t="shared" si="2"/>
+        <v>52.640000000000008</v>
+      </c>
+      <c r="M14" s="82">
+        <f t="shared" si="2"/>
+        <v>51.324000000000005</v>
+      </c>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4699,13 +5555,13 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:T11"/>
+  <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="16384" width="8.85546875" style="5"/>
   </cols>
@@ -4715,7 +5571,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="19.5" thickBot="1">
+    <row r="2" spans="2:20" ht="18.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>110</v>
       </c>
@@ -4796,411 +5652,635 @@
       <c r="S4" s="64"/>
       <c r="T4" s="64"/>
     </row>
-    <row r="5" spans="2:20" ht="19.5" thickBot="1">
+    <row r="5" spans="2:20" ht="18.75" thickBot="1">
       <c r="B5" s="65" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>56.4</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>45.9</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <v>23.5</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="29">
         <v>47.7</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <v>29.4</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>14.2</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="29">
         <v>47.9</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="29">
         <v>21.8</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="29">
         <v>24.6</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="29">
         <v>44.9</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="29">
         <v>31.1</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="29">
         <v>34.299999999999997</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="29">
         <v>48.2</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="29">
         <v>35.4</v>
       </c>
-      <c r="R5" s="30">
+      <c r="R5" s="29">
         <v>30.9</v>
       </c>
-      <c r="S5" s="30">
+      <c r="S5" s="29">
         <v>17.5</v>
       </c>
-      <c r="T5" s="30">
+      <c r="T5" s="29">
         <v>14.9</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="19.5" thickBot="1">
+    <row r="6" spans="2:20" ht="18.75" thickBot="1">
       <c r="B6" s="66"/>
       <c r="C6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>50.4</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>37.9</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <v>15.4</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>52.2</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="29">
         <v>27.5</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="29">
         <v>13.8</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="29">
         <v>47.6</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="29">
         <v>19.5</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="29">
         <v>17.8</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="29">
         <v>43.9</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="29">
         <v>26.5</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="29">
         <v>29</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="29">
         <v>47.9</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="29">
         <v>34.200000000000003</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R6" s="29">
         <v>30.2</v>
       </c>
-      <c r="S6" s="30">
+      <c r="S6" s="29">
         <v>13.1</v>
       </c>
-      <c r="T6" s="30">
+      <c r="T6" s="29">
         <v>11.3</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="19.5" thickBot="1">
+    <row r="7" spans="2:20" ht="18.75" thickBot="1">
       <c r="B7" s="67"/>
       <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>57.6</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>38.6</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <v>28</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="29">
         <v>50</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="29">
         <v>21.2</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>9.1</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="29">
         <v>43.9</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="29">
         <v>27.3</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="29">
         <v>22.7</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="29">
         <v>46.2</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="29">
         <v>34.1</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="29">
         <v>35.6</v>
       </c>
-      <c r="P7" s="30">
+      <c r="P7" s="29">
         <v>56.8</v>
       </c>
-      <c r="Q7" s="30">
+      <c r="Q7" s="29">
         <v>41.7</v>
       </c>
-      <c r="R7" s="30">
+      <c r="R7" s="29">
         <v>30.3</v>
       </c>
-      <c r="S7" s="30">
+      <c r="S7" s="29">
         <v>19.7</v>
       </c>
-      <c r="T7" s="30">
+      <c r="T7" s="29">
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="19.5" thickBot="1">
+    <row r="8" spans="2:20" ht="18.75" thickBot="1">
       <c r="B8" s="57" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>44.1</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>32.299999999999997</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <v>18</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="29">
         <v>55.3</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="29">
         <v>34.200000000000003</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>15.5</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="29">
         <v>42.9</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="29">
         <v>31.1</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="29">
         <v>17.399999999999999</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="29">
         <v>30.4</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="29">
         <v>28.6</v>
       </c>
-      <c r="O8" s="30">
+      <c r="O8" s="29">
         <v>20.5</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="29">
         <v>39.1</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="Q8" s="29">
         <v>27.3</v>
       </c>
-      <c r="R8" s="30">
+      <c r="R8" s="29">
         <v>25.5</v>
       </c>
-      <c r="S8" s="30">
+      <c r="S8" s="29">
         <v>11.8</v>
       </c>
-      <c r="T8" s="30">
+      <c r="T8" s="29">
         <v>9.9</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="19.5" thickBot="1">
+    <row r="9" spans="2:20" ht="18.75" thickBot="1">
       <c r="B9" s="58"/>
       <c r="C9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <v>53.1</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>41.9</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>20.5</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="29">
         <v>53</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="29">
         <v>28.6</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>14.4</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="29">
         <v>46.8</v>
       </c>
-      <c r="K9" s="30">
+      <c r="K9" s="29">
         <v>21.9</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="29">
         <v>19.5</v>
       </c>
-      <c r="M9" s="30">
+      <c r="M9" s="29">
         <v>44.8</v>
       </c>
-      <c r="N9" s="30">
+      <c r="N9" s="29">
         <v>27.8</v>
       </c>
-      <c r="O9" s="30">
+      <c r="O9" s="29">
         <v>29.7</v>
       </c>
-      <c r="P9" s="30">
+      <c r="P9" s="29">
         <v>47.4</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="Q9" s="29">
         <v>34.4</v>
       </c>
-      <c r="R9" s="30">
+      <c r="R9" s="29">
         <v>30.2</v>
       </c>
-      <c r="S9" s="30">
+      <c r="S9" s="29">
         <v>14</v>
       </c>
-      <c r="T9" s="30">
+      <c r="T9" s="29">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="19.5" thickBot="1">
+    <row r="10" spans="2:20" ht="18.75" thickBot="1">
       <c r="B10" s="58"/>
       <c r="C10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="29">
         <v>53.2</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>41</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <v>16.5</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <v>45.7</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="29">
         <v>26.4</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="29">
         <v>12.3</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="29">
         <v>51.2</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="29">
         <v>17.8</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="29">
         <v>24.1</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="29">
         <v>45</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="29">
         <v>31</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="29">
         <v>36.1</v>
       </c>
-      <c r="P10" s="30">
+      <c r="P10" s="29">
         <v>50.5</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="29">
         <v>36.799999999999997</v>
       </c>
-      <c r="R10" s="30">
+      <c r="R10" s="29">
         <v>32.700000000000003</v>
       </c>
-      <c r="S10" s="30">
+      <c r="S10" s="29">
         <v>16.8</v>
       </c>
-      <c r="T10" s="30">
+      <c r="T10" s="29">
         <v>15.2</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="19.5" thickBot="1">
+    <row r="11" spans="2:20" ht="18.75" thickBot="1">
       <c r="B11" s="59"/>
       <c r="C11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="29">
         <v>54.8</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>36.4</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <v>10.3</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="29">
         <v>30.1</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="29">
         <v>28.3</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="29">
         <v>14.7</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="29">
         <v>42.6</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="29">
         <v>11</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="29">
         <v>21.7</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M11" s="29">
         <v>40.799999999999997</v>
       </c>
-      <c r="N11" s="30">
+      <c r="N11" s="29">
         <v>27.2</v>
       </c>
-      <c r="O11" s="30">
+      <c r="O11" s="29">
         <v>35.299999999999997</v>
       </c>
-      <c r="P11" s="30">
+      <c r="P11" s="29">
         <v>51.8</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="29">
         <v>34.9</v>
       </c>
-      <c r="R11" s="30">
+      <c r="R11" s="29">
         <v>24.6</v>
       </c>
-      <c r="S11" s="30">
+      <c r="S11" s="29">
         <v>23.2</v>
       </c>
-      <c r="T11" s="30">
+      <c r="T11" s="29">
         <v>14.7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="82">
+        <f>(D5/100)*4424</f>
+        <v>2495.136</v>
+      </c>
+      <c r="E13" s="82">
+        <f t="shared" ref="E13:M13" si="0">(E5/100)*4424</f>
+        <v>2030.6159999999998</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="0"/>
+        <v>1039.6399999999999</v>
+      </c>
+      <c r="G13" s="82">
+        <f t="shared" si="0"/>
+        <v>2110.248</v>
+      </c>
+      <c r="H13" s="82">
+        <f t="shared" si="0"/>
+        <v>1300.6559999999999</v>
+      </c>
+      <c r="I13" s="82">
+        <f t="shared" si="0"/>
+        <v>628.20799999999997</v>
+      </c>
+      <c r="J13" s="82">
+        <f t="shared" si="0"/>
+        <v>2119.096</v>
+      </c>
+      <c r="K13" s="82">
+        <f t="shared" si="0"/>
+        <v>964.43200000000002</v>
+      </c>
+      <c r="L13" s="82">
+        <f t="shared" si="0"/>
+        <v>1088.3040000000001</v>
+      </c>
+      <c r="M13" s="82">
+        <f t="shared" si="0"/>
+        <v>1986.376</v>
+      </c>
+      <c r="N13" s="82">
+        <f t="shared" ref="N13:T13" si="1">(N5/100)*4424</f>
+        <v>1375.864</v>
+      </c>
+      <c r="O13" s="82">
+        <f t="shared" si="1"/>
+        <v>1517.4319999999998</v>
+      </c>
+      <c r="P13" s="82">
+        <f t="shared" si="1"/>
+        <v>2132.3680000000004</v>
+      </c>
+      <c r="Q13" s="82">
+        <f t="shared" si="1"/>
+        <v>1566.096</v>
+      </c>
+      <c r="R13" s="82">
+        <f t="shared" si="1"/>
+        <v>1367.0160000000001</v>
+      </c>
+      <c r="S13" s="82">
+        <f t="shared" si="1"/>
+        <v>774.19999999999993</v>
+      </c>
+      <c r="T13" s="82">
+        <f t="shared" si="1"/>
+        <v>659.17599999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20">
+      <c r="C14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="82">
+        <f>(D6/100)*5822</f>
+        <v>2934.288</v>
+      </c>
+      <c r="E14" s="82">
+        <f t="shared" ref="E14:M14" si="2">(E6/100)*5822</f>
+        <v>2206.538</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="2"/>
+        <v>896.58799999999997</v>
+      </c>
+      <c r="G14" s="82">
+        <f t="shared" si="2"/>
+        <v>3039.0840000000003</v>
+      </c>
+      <c r="H14" s="82">
+        <f t="shared" si="2"/>
+        <v>1601.0500000000002</v>
+      </c>
+      <c r="I14" s="82">
+        <f t="shared" si="2"/>
+        <v>803.43600000000004</v>
+      </c>
+      <c r="J14" s="82">
+        <f t="shared" si="2"/>
+        <v>2771.2720000000004</v>
+      </c>
+      <c r="K14" s="82">
+        <f t="shared" si="2"/>
+        <v>1135.29</v>
+      </c>
+      <c r="L14" s="82">
+        <f t="shared" si="2"/>
+        <v>1036.316</v>
+      </c>
+      <c r="M14" s="82">
+        <f t="shared" si="2"/>
+        <v>2555.8580000000002</v>
+      </c>
+      <c r="N14" s="82">
+        <f t="shared" ref="N14:T14" si="3">(N6/100)*5822</f>
+        <v>1542.8300000000002</v>
+      </c>
+      <c r="O14" s="82">
+        <f t="shared" si="3"/>
+        <v>1688.3799999999999</v>
+      </c>
+      <c r="P14" s="82">
+        <f t="shared" si="3"/>
+        <v>2788.7379999999998</v>
+      </c>
+      <c r="Q14" s="82">
+        <f t="shared" si="3"/>
+        <v>1991.1240000000003</v>
+      </c>
+      <c r="R14" s="82">
+        <f t="shared" si="3"/>
+        <v>1758.2439999999999</v>
+      </c>
+      <c r="S14" s="82">
+        <f t="shared" si="3"/>
+        <v>762.68200000000002</v>
+      </c>
+      <c r="T14" s="82">
+        <f t="shared" si="3"/>
+        <v>657.88599999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20">
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="82">
+        <f>(D7/100)*188</f>
+        <v>108.28800000000001</v>
+      </c>
+      <c r="E15" s="82">
+        <f t="shared" ref="E15:M15" si="4">(E7/100)*188</f>
+        <v>72.567999999999998</v>
+      </c>
+      <c r="F15" s="82">
+        <f t="shared" si="4"/>
+        <v>52.640000000000008</v>
+      </c>
+      <c r="G15" s="82">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="H15" s="82">
+        <f t="shared" si="4"/>
+        <v>39.856000000000002</v>
+      </c>
+      <c r="I15" s="82">
+        <f t="shared" si="4"/>
+        <v>17.108000000000001</v>
+      </c>
+      <c r="J15" s="82">
+        <f t="shared" si="4"/>
+        <v>82.531999999999996</v>
+      </c>
+      <c r="K15" s="82">
+        <f t="shared" si="4"/>
+        <v>51.324000000000005</v>
+      </c>
+      <c r="L15" s="82">
+        <f t="shared" si="4"/>
+        <v>42.675999999999995</v>
+      </c>
+      <c r="M15" s="82">
+        <f t="shared" si="4"/>
+        <v>86.856000000000009</v>
+      </c>
+      <c r="N15" s="82">
+        <f t="shared" ref="N15:T15" si="5">(N7/100)*188</f>
+        <v>64.108000000000004</v>
+      </c>
+      <c r="O15" s="82">
+        <f t="shared" si="5"/>
+        <v>66.928000000000011</v>
+      </c>
+      <c r="P15" s="82">
+        <f t="shared" si="5"/>
+        <v>106.78399999999999</v>
+      </c>
+      <c r="Q15" s="82">
+        <f t="shared" si="5"/>
+        <v>78.396000000000001</v>
+      </c>
+      <c r="R15" s="82">
+        <f t="shared" si="5"/>
+        <v>56.963999999999999</v>
+      </c>
+      <c r="S15" s="82">
+        <f t="shared" si="5"/>
+        <v>37.035999999999994</v>
+      </c>
+      <c r="T15" s="82">
+        <f t="shared" si="5"/>
+        <v>32.711999999999996</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="B5:B7"/>
@@ -5216,11 +6296,6 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>